<commit_message>
Cambio lectura matriz, ahora desde JSON
</commit_message>
<xml_diff>
--- a/pytasks/Formatos/MATRIZ TASACIONES.xlsx
+++ b/pytasks/Formatos/MATRIZ TASACIONES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pollo\OneDrive\Development\1- Bienes Futuros\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pollo\OneDrive\Development\1-BienesFuturos\pytasks\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29851D06-F97C-4E15-B550-4E805247D9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0E90B6-E655-49F4-9F12-B3811943667E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2055" windowWidth="21600" windowHeight="11505" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRIZ" sheetId="3" r:id="rId1"/>
@@ -35,64 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andrés Ernesto Gómez Garcés</author>
-  </authors>
-  <commentList>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{68481D6E-576F-40B0-B7FE-99F4BE2ABD50}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Ernesto Gómez Garcés:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-opción de inclusión de pocentaje de cálculo con % adicional a la minuta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{B35969C7-D9AF-4CBB-A3E9-7E756AD2DD5A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Ernesto Gómez Garcés:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Factor desde 1.15 - 1.4 dependiendo del tipo de proyecto</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
@@ -252,7 +194,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,19 +236,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -915,7 +844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="sh3Matriz">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -926,7 +855,7 @@
       <selection activeCell="AA81" sqref="AA81"/>
       <selection pane="topRight" activeCell="AA81" sqref="AA81"/>
       <selection pane="bottomLeft" activeCell="AA81" sqref="AA81"/>
-      <selection pane="bottomRight" activeCell="S12" sqref="S12"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1377,6 @@
   <headerFooter scaleWithDoc="0">
     <oddHeader>&amp;L&amp;G&amp;R&amp;"Verdana,Normal"&amp;8&amp;K00-024Página &amp;P de &amp;N</oddHeader>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-  <legacyDrawingHF r:id="rId3"/>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>